<commit_message>
Fix: use TEMPLATE_PATH in compare_excels + bundle template
</commit_message>
<xml_diff>
--- a/data/Fichier_Excel_Professeur_Template.xlsx
+++ b/data/Fichier_Excel_Professeur_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youss\Downloads\Stage 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chaima\Downloads\smartedittrack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5ED399-3AF8-4E2F-AD91-4BB2C9C95560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1127F-A391-4D3A-B63A-1E341CDEF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Prénom</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>Q4 - Donner l’expression de σmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> formé de béton et d’armatures en acie</t>
+  </si>
+  <si>
+    <t>σ = N / A</t>
+  </si>
+  <si>
+    <t>σmax = M × y / I</t>
+  </si>
+  <si>
+    <t>M = σ × W (ou M = E × I × κ). Ia</t>
   </si>
 </sst>
 </file>
@@ -402,22 +414,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:G1"/>
+  <dimension ref="C1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
-    <col min="7" max="7" width="49.44140625" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,6 +444,20 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>